<commit_message>
(!!!) Working T4_horizontalbar + Added percentages to T4
</commit_message>
<xml_diff>
--- a/data/excel/T4.xlsx
+++ b/data/excel/T4.xlsx
@@ -2,13 +2,13 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28025"/>
-  <workbookPr defaultThemeVersion="202300"/>
+  <workbookPr hidePivotFieldList="1" defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Vincent\Downloads\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Vincent\Documents\GitHub\Data-Visualisation-2\data\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{CF48DB8B-041B-407E-BF38-E530F31CA6DB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0C13042A-98B1-48DB-AE84-E2E1A4D10E1E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{D373851B-B6E4-4A1C-88F7-447150AE332B}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="16">
   <si>
     <t>Gender</t>
   </si>
@@ -81,6 +81,9 @@
   </si>
   <si>
     <t>Female</t>
+  </si>
+  <si>
+    <t>Percentage</t>
   </si>
 </sst>
 </file>
@@ -461,18 +464,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{565A8EF6-4D1A-4123-9DE6-AE4D8A2069DA}">
-  <dimension ref="A1:C21"/>
+  <dimension ref="A1:D21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E15" sqref="E15"/>
+      <selection activeCell="L12" sqref="L12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="43.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="18.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -482,8 +486,11 @@
       <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D1" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>13</v>
       </c>
@@ -493,8 +500,11 @@
       <c r="C2">
         <v>349430</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D2">
+        <v>74.295907909900023</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>13</v>
       </c>
@@ -504,8 +514,11 @@
       <c r="C3">
         <v>1641014</v>
       </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D3">
+        <v>91.560186778955739</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>13</v>
       </c>
@@ -515,8 +528,11 @@
       <c r="C4">
         <v>629035</v>
       </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D4">
+        <v>89.483117936170359</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>13</v>
       </c>
@@ -526,8 +542,11 @@
       <c r="C5">
         <v>170111</v>
       </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D5">
+        <v>68.11196707133476</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>13</v>
       </c>
@@ -537,8 +556,11 @@
       <c r="C6">
         <v>313534</v>
       </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D6">
+        <v>23.123170075151371</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>13</v>
       </c>
@@ -548,8 +570,11 @@
       <c r="C7">
         <v>231740</v>
       </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D7">
+        <v>22.711324889354078</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>13</v>
       </c>
@@ -559,8 +584,11 @@
       <c r="C8">
         <v>1064793</v>
       </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D8">
+        <v>41.45269930945453</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>13</v>
       </c>
@@ -570,8 +598,11 @@
       <c r="C9">
         <v>506840</v>
       </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D9">
+        <v>31.806834540952146</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>13</v>
       </c>
@@ -581,8 +612,11 @@
       <c r="C10">
         <v>203629</v>
       </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D10">
+        <v>40.12449432800058</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>13</v>
       </c>
@@ -592,8 +626,11 @@
       <c r="C11">
         <v>231733</v>
       </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D11">
+        <v>36.320819037737238</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>14</v>
       </c>
@@ -603,8 +640,11 @@
       <c r="C12">
         <v>120892</v>
       </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D12">
+        <v>25.704092090099973</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>14</v>
       </c>
@@ -614,8 +654,11 @@
       <c r="C13">
         <v>151265</v>
       </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D13">
+        <v>8.4398132210442682</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>14</v>
       </c>
@@ -625,8 +668,11 @@
       <c r="C14">
         <v>73930</v>
       </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D14">
+        <v>10.516882063829636</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>14</v>
       </c>
@@ -636,8 +682,11 @@
       <c r="C15">
         <v>79641</v>
       </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D15">
+        <v>31.888032928665233</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>14</v>
       </c>
@@ -647,8 +696,11 @@
       <c r="C16">
         <v>1042396</v>
       </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D16">
+        <v>76.876829924848636</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>14</v>
       </c>
@@ -658,8 +710,11 @@
       <c r="C17">
         <v>788632</v>
       </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D17">
+        <v>77.288675110645926</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>14</v>
       </c>
@@ -669,8 +724,11 @@
       <c r="C18">
         <v>1503901</v>
       </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D18">
+        <v>58.54730069054547</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>14</v>
       </c>
@@ -680,8 +738,11 @@
       <c r="C19">
         <v>1086654</v>
       </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D19">
+        <v>68.193165459047862</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>14</v>
       </c>
@@ -691,8 +752,11 @@
       <c r="C20">
         <v>303864</v>
       </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D20">
+        <v>59.87550567199942</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>14</v>
       </c>
@@ -701,6 +765,9 @@
       </c>
       <c r="C21">
         <v>406284</v>
+      </c>
+      <c r="D21">
+        <v>63.679180962262762</v>
       </c>
     </row>
   </sheetData>

</xml_diff>